<commit_message>
manuscript figures and tables
</commit_message>
<xml_diff>
--- a/manuscript/tables/conversion-locher.xlsx
+++ b/manuscript/tables/conversion-locher.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/phd/manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7098B9BC-37D9-3E43-A3D7-16F45241289A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACF3CD8-1965-EF48-9246-E21160AD8F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{171DD23E-46AE-504D-BDCD-0CA54D12CF71}"/>
   </bookViews>
@@ -36,48 +36,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Locher's subgroup</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>CAZy clan</t>
   </si>
   <si>
-    <t>GT-CA</t>
-  </si>
-  <si>
-    <t>GT-CB</t>
+    <t>CAZy families</t>
+  </si>
+  <si>
+    <t>X586, X606, X608, X610, X611, X612</t>
+  </si>
+  <si>
+    <t>X605, X607, X609, X613, X614, X615</t>
+  </si>
+  <si>
+    <t>Structural subclass Locher</t>
+  </si>
+  <si>
+    <t>GT-CB2</t>
+  </si>
+  <si>
+    <t>GT-CB1</t>
+  </si>
+  <si>
+    <t>X571</t>
+  </si>
+  <si>
+    <t>X617</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>GT-C1</t>
-  </si>
-  <si>
-    <t>GT-C2</t>
-  </si>
-  <si>
-    <t>GT-C3</t>
-  </si>
-  <si>
-    <t>GT-C4</t>
-  </si>
-  <si>
-    <t>CAZy families</t>
-  </si>
-  <si>
-    <t>GT66, GT83, GT39, GT57, GT53</t>
-  </si>
-  <si>
-    <t>X571, X605, X607, X609, X613, X614, X615</t>
-  </si>
-  <si>
-    <t>X586, X606, X608, X610, X611, X612</t>
-  </si>
-  <si>
-    <t>X617</t>
+    <t>GT-CA (7 conserved)</t>
+  </si>
+  <si>
+    <t>GT-CB (10 conserved)</t>
+  </si>
+  <si>
+    <t>GT66</t>
+  </si>
+  <si>
+    <t>GT83</t>
+  </si>
+  <si>
+    <t>GT39</t>
+  </si>
+  <si>
+    <t>GT57</t>
+  </si>
+  <si>
+    <t>GT53</t>
+  </si>
+  <si>
+    <t>Activator</t>
+  </si>
+  <si>
+    <t>Lipid-P</t>
+  </si>
+  <si>
+    <t>GT22</t>
+  </si>
+  <si>
+    <t>GT50</t>
+  </si>
+  <si>
+    <t>GT58</t>
+  </si>
+  <si>
+    <t>GT59</t>
+  </si>
+  <si>
+    <t>Inverting</t>
+  </si>
+  <si>
+    <t>Retaining</t>
+  </si>
+  <si>
+    <t>Lipid-PP-oligosaccharide</t>
   </si>
 </sst>
 </file>
@@ -119,8 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,70 +474,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2623CA1E-152F-564F-AC63-B2698A471404}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>